<commit_message>
Download item_master excel is now downlodable
</commit_message>
<xml_diff>
--- a/src/Assets/Data/Files/item_master.xlsx
+++ b/src/Assets/Data/Files/item_master.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">hsn_code</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">sgst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stock</t>
   </si>
   <si>
     <t xml:space="preserve">Apple</t>
@@ -174,13 +171,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -204,16 +201,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>987640</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
@@ -229,9 +223,6 @@
       </c>
       <c r="G2" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,7 +230,7 @@
         <v>897651</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -255,9 +246,6 @@
       </c>
       <c r="G3" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,7 +253,7 @@
         <v>465643</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -281,9 +269,6 @@
       </c>
       <c r="G4" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,7 +276,7 @@
         <v>537527</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0</v>
@@ -307,9 +292,6 @@
       </c>
       <c r="G5" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,7 +299,7 @@
         <v>885232</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0</v>
@@ -333,9 +315,6 @@
       </c>
       <c r="G6" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,7 +322,7 @@
         <v>578424</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
@@ -359,9 +338,6 @@
       </c>
       <c r="G7" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,7 +345,7 @@
         <v>527876</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
@@ -385,9 +361,6 @@
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,7 +368,7 @@
         <v>978554</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
@@ -411,9 +384,6 @@
       </c>
       <c r="G9" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,7 +391,7 @@
         <v>741223</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -437,9 +407,6 @@
       </c>
       <c r="G10" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,7 +414,7 @@
         <v>124486</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
@@ -463,9 +430,6 @@
       </c>
       <c r="G11" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>